<commit_message>
shop 데이터 notice, intro NULL로 수정
</commit_message>
<xml_diff>
--- a/realtime_shop_data.xlsx
+++ b/realtime_shop_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="174">
   <si>
     <t>telephone</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -607,6 +607,10 @@
   </si>
   <si>
     <t>media/2022/03/02/fromis9.jpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Null</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1260,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1459,7 +1463,9 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3" s="19"/>
+      <c r="P3" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="Q3" s="31" t="s">
         <v>160</v>
       </c>
@@ -1522,7 +1528,9 @@
       <c r="P4" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="Q4" s="23"/>
+      <c r="Q4" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S4" s="29">
         <v>44619.740624942133</v>
       </c>
@@ -1582,7 +1590,9 @@
       <c r="P5" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="Q5" s="23"/>
+      <c r="Q5" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S5" s="29">
         <v>44620.740624942133</v>
       </c>
@@ -1642,7 +1652,9 @@
       <c r="P6" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="Q6" s="23"/>
+      <c r="Q6" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S6" s="29">
         <v>44621.740624942133</v>
       </c>
@@ -1885,8 +1897,12 @@
       <c r="O10">
         <v>1</v>
       </c>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="23"/>
+      <c r="P10" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="R10" s="33" t="s">
         <v>172</v>
       </c>
@@ -1946,8 +1962,12 @@
       <c r="O11">
         <v>1</v>
       </c>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="23"/>
+      <c r="P11" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q11" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S11" s="29">
         <v>44626.740624942133</v>
       </c>
@@ -2004,8 +2024,12 @@
       <c r="O12">
         <v>1</v>
       </c>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="23"/>
+      <c r="P12" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S12" s="29">
         <v>44627.740624942133</v>
       </c>
@@ -2065,7 +2089,9 @@
       <c r="P13" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="Q13" s="23"/>
+      <c r="Q13" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S13" s="29">
         <v>44628.740624942133</v>
       </c>
@@ -2122,8 +2148,12 @@
       <c r="O14">
         <v>1</v>
       </c>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="23"/>
+      <c r="P14" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q14" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S14" s="29">
         <v>44629.740624942133</v>
       </c>
@@ -2180,8 +2210,12 @@
       <c r="O15">
         <v>1</v>
       </c>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="23"/>
+      <c r="P15" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q15" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S15" s="29">
         <v>44630.740624942133</v>
       </c>
@@ -2238,8 +2272,12 @@
       <c r="O16">
         <v>1</v>
       </c>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="23"/>
+      <c r="P16" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q16" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S16" s="29">
         <v>44631.740624942133</v>
       </c>
@@ -2296,8 +2334,12 @@
       <c r="O17">
         <v>1</v>
       </c>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="23"/>
+      <c r="P17" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q17" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S17" s="29">
         <v>44632.740624942133</v>
       </c>
@@ -2416,8 +2458,12 @@
       <c r="O19">
         <v>1</v>
       </c>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="23"/>
+      <c r="P19" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q19" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="S19" s="29">
         <v>44634.740624942133</v>
       </c>
@@ -2599,7 +2645,7 @@
         <v>1</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="Q22" s="31" t="s">
         <v>162</v>

</xml_diff>